<commit_message>
added p chart, improved readability, bug fixes for anomaly detection
</commit_message>
<xml_diff>
--- a/assets/sample_data.xlsx
+++ b/assets/sample_data.xlsx
@@ -9,14 +9,13 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="17256" windowHeight="7812" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="17256" windowHeight="7812" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="set_1" sheetId="1" r:id="rId1"/>
     <sheet name="set_2" sheetId="4" r:id="rId2"/>
-    <sheet name="set_3" sheetId="5" r:id="rId3"/>
-    <sheet name="set_4" sheetId="2" r:id="rId4"/>
-    <sheet name="set_5" sheetId="3" r:id="rId5"/>
+    <sheet name="set_3" sheetId="2" r:id="rId3"/>
+    <sheet name="set_4" sheetId="3" r:id="rId4"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -28,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="2">
   <si>
     <t>Sample</t>
   </si>
@@ -692,15 +691,15 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F26"/>
+  <dimension ref="A1:H12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+      <selection activeCell="J10" sqref="J10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -719,506 +718,279 @@
       <c r="F1">
         <v>5</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G1">
+        <v>6</v>
+      </c>
+      <c r="H1">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2" s="2">
-        <v>20</v>
+        <v>35.9</v>
       </c>
       <c r="C2" s="2">
-        <v>22</v>
+        <v>35.5</v>
       </c>
       <c r="D2" s="2">
-        <v>21</v>
+        <v>34.1</v>
       </c>
       <c r="E2" s="2">
-        <v>23</v>
+        <v>34.1</v>
       </c>
       <c r="F2" s="2">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+        <v>35.799999999999997</v>
+      </c>
+      <c r="G2" s="2">
+        <v>37.1</v>
+      </c>
+      <c r="H2" s="2">
+        <v>35.1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3" s="2">
-        <v>19</v>
+        <v>34.299999999999997</v>
       </c>
       <c r="C3" s="2">
-        <v>18</v>
+        <v>35</v>
       </c>
       <c r="D3" s="2">
-        <v>22</v>
+        <v>37.4</v>
       </c>
       <c r="E3" s="2">
-        <v>20</v>
+        <v>35.200000000000003</v>
       </c>
       <c r="F3" s="2">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+        <v>35.5</v>
+      </c>
+      <c r="G3" s="2">
+        <v>35.4</v>
+      </c>
+      <c r="H3" s="2">
+        <v>35.299999999999997</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>3</v>
       </c>
       <c r="B4" s="2">
-        <v>25</v>
+        <v>32.6</v>
       </c>
       <c r="C4" s="2">
-        <v>18</v>
+        <v>35.200000000000003</v>
       </c>
       <c r="D4" s="2">
-        <v>20</v>
+        <v>34.6</v>
       </c>
       <c r="E4" s="2">
-        <v>17</v>
+        <v>30.7</v>
       </c>
       <c r="F4" s="2">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+        <v>35.200000000000003</v>
+      </c>
+      <c r="G4" s="2">
+        <v>37</v>
+      </c>
+      <c r="H4" s="2">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>4</v>
       </c>
       <c r="B5" s="2">
-        <v>20</v>
+        <v>34.200000000000003</v>
       </c>
       <c r="C5" s="2">
-        <v>21</v>
+        <v>36.200000000000003</v>
       </c>
       <c r="D5" s="2">
-        <v>22</v>
+        <v>35.5</v>
       </c>
       <c r="E5" s="2">
-        <v>21</v>
+        <v>36.9</v>
       </c>
       <c r="F5" s="2">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+        <v>34.299999999999997</v>
+      </c>
+      <c r="G5" s="2">
+        <v>34.200000000000003</v>
+      </c>
+      <c r="H5" s="2">
+        <v>36.200000000000003</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>5</v>
       </c>
       <c r="B6" s="2">
-        <v>19</v>
+        <v>35.9</v>
       </c>
       <c r="C6" s="2">
-        <v>24</v>
+        <v>35</v>
       </c>
       <c r="D6" s="2">
-        <v>23</v>
+        <v>34</v>
       </c>
       <c r="E6" s="2">
-        <v>22</v>
+        <v>37.9</v>
       </c>
       <c r="F6" s="2">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+        <v>32.799999999999997</v>
+      </c>
+      <c r="G6" s="2">
+        <v>34.4</v>
+      </c>
+      <c r="H6" s="2">
+        <v>33.4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>6</v>
       </c>
       <c r="B7" s="2">
-        <v>22</v>
+        <v>35.700000000000003</v>
       </c>
       <c r="C7" s="2">
-        <v>20</v>
+        <v>35.200000000000003</v>
       </c>
       <c r="D7" s="2">
-        <v>18</v>
+        <v>34.799999999999997</v>
       </c>
       <c r="E7" s="2">
-        <v>18</v>
+        <v>33.700000000000003</v>
       </c>
       <c r="F7" s="2">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+        <v>35.200000000000003</v>
+      </c>
+      <c r="G7" s="2">
+        <v>36.6</v>
+      </c>
+      <c r="H7" s="2">
+        <v>35.299999999999997</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>7</v>
       </c>
       <c r="B8" s="2">
-        <v>18</v>
+        <v>35</v>
       </c>
       <c r="C8" s="2">
-        <v>20</v>
+        <v>35.5</v>
       </c>
       <c r="D8" s="2">
-        <v>19</v>
+        <v>36.200000000000003</v>
       </c>
       <c r="E8" s="2">
-        <v>18</v>
+        <v>32.6</v>
       </c>
       <c r="F8" s="2">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+        <v>36.5</v>
+      </c>
+      <c r="G8" s="2">
+        <v>33.6</v>
+      </c>
+      <c r="H8" s="2">
+        <v>35.4</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>8</v>
       </c>
       <c r="B9" s="2">
-        <v>20</v>
+        <v>37</v>
       </c>
       <c r="C9" s="2">
-        <v>18</v>
+        <v>35.299999999999997</v>
       </c>
       <c r="D9" s="2">
-        <v>23</v>
+        <v>34.5</v>
       </c>
       <c r="E9" s="2">
-        <v>20</v>
+        <v>34.1</v>
       </c>
       <c r="F9" s="2">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+        <v>36.4</v>
+      </c>
+      <c r="G9" s="2">
+        <v>35.9</v>
+      </c>
+      <c r="H9" s="2">
+        <v>37.6</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>9</v>
       </c>
       <c r="B10" s="2">
-        <v>21</v>
+        <v>34.700000000000003</v>
       </c>
       <c r="C10" s="2">
-        <v>20</v>
+        <v>34.700000000000003</v>
       </c>
       <c r="D10" s="2">
-        <v>24</v>
+        <v>36.200000000000003</v>
       </c>
       <c r="E10" s="2">
-        <v>23</v>
+        <v>34.700000000000003</v>
       </c>
       <c r="F10" s="2">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+        <v>34.700000000000003</v>
+      </c>
+      <c r="G10" s="2">
+        <v>37.9</v>
+      </c>
+      <c r="H10" s="2">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>10</v>
       </c>
       <c r="B11" s="2">
-        <v>21</v>
+        <v>35.1</v>
       </c>
       <c r="C11" s="2">
-        <v>19</v>
+        <v>35.5</v>
       </c>
       <c r="D11" s="2">
-        <v>20</v>
+        <v>35</v>
       </c>
       <c r="E11" s="2">
-        <v>20</v>
+        <v>36.1</v>
       </c>
       <c r="F11" s="2">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A12">
-        <v>11</v>
-      </c>
-      <c r="B12" s="2">
-        <v>20</v>
-      </c>
-      <c r="C12" s="2">
-        <v>20</v>
-      </c>
-      <c r="D12" s="2">
-        <v>23</v>
-      </c>
-      <c r="E12" s="2">
-        <v>22</v>
-      </c>
-      <c r="F12" s="2">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A13">
-        <v>12</v>
-      </c>
-      <c r="B13" s="2">
-        <v>22</v>
-      </c>
-      <c r="C13" s="2">
-        <v>21</v>
-      </c>
-      <c r="D13" s="2">
-        <v>20</v>
-      </c>
-      <c r="E13" s="2">
-        <v>22</v>
-      </c>
-      <c r="F13" s="2">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A14">
-        <v>13</v>
-      </c>
-      <c r="B14" s="2">
-        <v>19</v>
-      </c>
-      <c r="C14" s="2">
-        <v>22</v>
-      </c>
-      <c r="D14" s="2">
-        <v>19</v>
-      </c>
-      <c r="E14" s="2">
-        <v>18</v>
-      </c>
-      <c r="F14" s="2">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A15">
-        <v>14</v>
-      </c>
-      <c r="B15" s="2">
-        <v>20</v>
-      </c>
-      <c r="C15" s="2">
-        <v>21</v>
-      </c>
-      <c r="D15" s="2">
-        <v>22</v>
-      </c>
-      <c r="E15" s="2">
-        <v>21</v>
-      </c>
-      <c r="F15" s="2">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A16">
-        <v>15</v>
-      </c>
-      <c r="B16" s="2">
-        <v>20</v>
-      </c>
-      <c r="C16" s="2">
-        <v>24</v>
-      </c>
-      <c r="D16" s="2">
-        <v>24</v>
-      </c>
-      <c r="E16" s="2">
-        <v>23</v>
-      </c>
-      <c r="F16" s="2">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A17">
-        <v>16</v>
-      </c>
-      <c r="B17" s="2">
-        <v>21</v>
-      </c>
-      <c r="C17" s="2">
-        <v>20</v>
-      </c>
-      <c r="D17" s="2">
-        <v>24</v>
-      </c>
-      <c r="E17" s="2">
-        <v>20</v>
-      </c>
-      <c r="F17" s="2">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A18">
-        <v>17</v>
-      </c>
-      <c r="B18" s="2">
-        <v>20</v>
-      </c>
-      <c r="C18" s="2">
-        <v>18</v>
-      </c>
-      <c r="D18" s="2">
-        <v>18</v>
-      </c>
-      <c r="E18" s="2">
-        <v>20</v>
-      </c>
-      <c r="F18" s="2">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A19">
-        <v>18</v>
-      </c>
-      <c r="B19" s="2">
-        <v>20</v>
-      </c>
-      <c r="C19" s="2">
-        <v>24</v>
-      </c>
-      <c r="D19" s="2">
-        <v>22</v>
-      </c>
-      <c r="E19" s="2">
-        <v>23</v>
-      </c>
-      <c r="F19" s="2">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A20">
-        <v>19</v>
-      </c>
-      <c r="B20" s="2">
-        <v>20</v>
-      </c>
-      <c r="C20" s="2">
-        <v>19</v>
-      </c>
-      <c r="D20" s="2">
-        <v>23</v>
-      </c>
-      <c r="E20" s="2">
-        <v>20</v>
-      </c>
-      <c r="F20" s="2">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A21">
-        <v>20</v>
-      </c>
-      <c r="B21" s="2">
-        <v>22</v>
-      </c>
-      <c r="C21" s="2">
-        <v>21</v>
-      </c>
-      <c r="D21" s="2">
-        <v>21</v>
-      </c>
-      <c r="E21" s="2">
-        <v>24</v>
-      </c>
-      <c r="F21" s="2">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A22">
-        <v>21</v>
-      </c>
-      <c r="B22" s="2">
-        <v>23</v>
-      </c>
-      <c r="C22" s="2">
-        <v>22</v>
-      </c>
-      <c r="D22" s="2">
-        <v>22</v>
-      </c>
-      <c r="E22" s="2">
-        <v>20</v>
-      </c>
-      <c r="F22" s="2">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A23">
-        <v>22</v>
-      </c>
-      <c r="B23" s="2">
-        <v>21</v>
-      </c>
-      <c r="C23" s="2">
-        <v>18</v>
-      </c>
-      <c r="D23" s="2">
-        <v>18</v>
-      </c>
-      <c r="E23" s="2">
-        <v>17</v>
-      </c>
-      <c r="F23" s="2">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A24">
-        <v>23</v>
-      </c>
-      <c r="B24" s="2">
-        <v>21</v>
-      </c>
-      <c r="C24" s="2">
-        <v>24</v>
-      </c>
-      <c r="D24" s="2">
-        <v>24</v>
-      </c>
-      <c r="E24" s="2">
-        <v>23</v>
-      </c>
-      <c r="F24" s="2">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A25">
-        <v>24</v>
-      </c>
-      <c r="B25" s="2">
-        <v>20</v>
-      </c>
-      <c r="C25" s="2">
-        <v>22</v>
-      </c>
-      <c r="D25" s="2">
-        <v>21</v>
-      </c>
-      <c r="E25" s="2">
-        <v>21</v>
-      </c>
-      <c r="F25" s="2">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A26">
-        <v>25</v>
-      </c>
-      <c r="B26" s="2">
-        <v>19</v>
-      </c>
-      <c r="C26" s="2">
-        <v>20</v>
-      </c>
-      <c r="D26" s="2">
-        <v>21</v>
-      </c>
-      <c r="E26" s="2">
-        <v>21</v>
-      </c>
-      <c r="F26" s="2">
-        <v>22</v>
-      </c>
+        <v>31.1</v>
+      </c>
+      <c r="G11" s="2">
+        <v>34.4</v>
+      </c>
+      <c r="H11" s="2">
+        <v>35.4</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="B12" s="2"/>
+      <c r="C12" s="2"/>
+      <c r="D12" s="2"/>
+      <c r="E12" s="2"/>
+      <c r="F12" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1227,189 +999,6 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B21"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C31" sqref="C31"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A2">
-        <v>1</v>
-      </c>
-      <c r="B2">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A3">
-        <v>2</v>
-      </c>
-      <c r="B3">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A4">
-        <v>3</v>
-      </c>
-      <c r="B4">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A5">
-        <v>4</v>
-      </c>
-      <c r="B5">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A6">
-        <v>5</v>
-      </c>
-      <c r="B6">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A7">
-        <v>6</v>
-      </c>
-      <c r="B7">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A8">
-        <v>7</v>
-      </c>
-      <c r="B8">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A9">
-        <v>8</v>
-      </c>
-      <c r="B9">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A10">
-        <v>9</v>
-      </c>
-      <c r="B10">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A11">
-        <v>10</v>
-      </c>
-      <c r="B11">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A12">
-        <v>11</v>
-      </c>
-      <c r="B12">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A13">
-        <v>12</v>
-      </c>
-      <c r="B13">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A14">
-        <v>13</v>
-      </c>
-      <c r="B14">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A15">
-        <v>14</v>
-      </c>
-      <c r="B15">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A16">
-        <v>15</v>
-      </c>
-      <c r="B16">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A17">
-        <v>16</v>
-      </c>
-      <c r="B17">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A18">
-        <v>17</v>
-      </c>
-      <c r="B18">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A19">
-        <v>18</v>
-      </c>
-      <c r="B19">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A20">
-        <v>19</v>
-      </c>
-      <c r="B20">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A21">
-        <v>20</v>
-      </c>
-      <c r="B21">
-        <v>21</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B11"/>
   <sheetViews>
@@ -1512,12 +1101,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
updated anomaly detection, added XmR
</commit_message>
<xml_diff>
--- a/assets/sample_data.xlsx
+++ b/assets/sample_data.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="17256" windowHeight="7812" activeTab="5"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="17256" windowHeight="7812" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="set_1" sheetId="1" r:id="rId1"/>
@@ -360,7 +360,7 @@
   <dimension ref="A1:F16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:B1"/>
+      <selection activeCell="C23" sqref="C23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -693,10 +693,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H12"/>
+  <dimension ref="A1:H21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J10" sqref="J10"/>
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -717,282 +717,377 @@
       <c r="E1">
         <v>4</v>
       </c>
-      <c r="F1">
-        <v>5</v>
-      </c>
-      <c r="G1">
-        <v>6</v>
-      </c>
-      <c r="H1">
-        <v>7</v>
-      </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2" s="2">
-        <v>35.9</v>
+        <v>44.01</v>
       </c>
       <c r="C2" s="2">
-        <v>35.5</v>
+        <v>26</v>
       </c>
       <c r="D2" s="2">
-        <v>34.1</v>
+        <v>24</v>
       </c>
       <c r="E2" s="2">
-        <v>34.1</v>
-      </c>
-      <c r="F2" s="2">
-        <v>35.799999999999997</v>
-      </c>
-      <c r="G2" s="2">
-        <v>37.1</v>
-      </c>
-      <c r="H2" s="2">
-        <v>35.1</v>
-      </c>
+        <v>34</v>
+      </c>
+      <c r="F2" s="2"/>
+      <c r="G2" s="2"/>
+      <c r="H2" s="2"/>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3" s="2">
-        <v>34.299999999999997</v>
+        <v>50</v>
       </c>
       <c r="C3" s="2">
-        <v>35</v>
+        <v>48</v>
       </c>
       <c r="D3" s="2">
-        <v>37.4</v>
+        <v>51</v>
       </c>
       <c r="E3" s="2">
-        <v>35.200000000000003</v>
-      </c>
-      <c r="F3" s="2">
-        <v>35.5</v>
-      </c>
-      <c r="G3" s="2">
-        <v>35.4</v>
-      </c>
-      <c r="H3" s="2">
-        <v>35.299999999999997</v>
-      </c>
+        <v>43</v>
+      </c>
+      <c r="F3" s="2"/>
+      <c r="G3" s="2"/>
+      <c r="H3" s="2"/>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>3</v>
       </c>
       <c r="B4" s="2">
-        <v>32.6</v>
+        <v>32</v>
       </c>
       <c r="C4" s="2">
-        <v>35.200000000000003</v>
+        <v>28</v>
       </c>
       <c r="D4" s="2">
-        <v>34.6</v>
+        <v>26</v>
       </c>
       <c r="E4" s="2">
-        <v>30.7</v>
-      </c>
-      <c r="F4" s="2">
-        <v>35.200000000000003</v>
-      </c>
-      <c r="G4" s="2">
-        <v>37</v>
-      </c>
-      <c r="H4" s="2">
-        <v>33</v>
-      </c>
+        <v>22</v>
+      </c>
+      <c r="F4" s="2"/>
+      <c r="G4" s="2"/>
+      <c r="H4" s="2"/>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>4</v>
       </c>
       <c r="B5" s="2">
-        <v>34.200000000000003</v>
+        <v>52</v>
       </c>
       <c r="C5" s="2">
-        <v>36.200000000000003</v>
+        <v>55</v>
       </c>
       <c r="D5" s="2">
-        <v>35.5</v>
+        <v>56</v>
       </c>
       <c r="E5" s="2">
-        <v>36.9</v>
-      </c>
-      <c r="F5" s="2">
-        <v>34.299999999999997</v>
-      </c>
-      <c r="G5" s="2">
-        <v>34.200000000000003</v>
-      </c>
-      <c r="H5" s="2">
-        <v>36.200000000000003</v>
-      </c>
+        <v>44</v>
+      </c>
+      <c r="F5" s="2"/>
+      <c r="G5" s="2"/>
+      <c r="H5" s="2"/>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>5</v>
       </c>
       <c r="B6" s="2">
-        <v>35.9</v>
+        <v>16</v>
       </c>
       <c r="C6" s="2">
-        <v>35</v>
+        <v>16</v>
       </c>
       <c r="D6" s="2">
-        <v>34</v>
+        <v>21</v>
       </c>
       <c r="E6" s="2">
-        <v>37.9</v>
-      </c>
-      <c r="F6" s="2">
-        <v>32.799999999999997</v>
-      </c>
-      <c r="G6" s="2">
-        <v>34.4</v>
-      </c>
-      <c r="H6" s="2">
-        <v>33.4</v>
-      </c>
+        <v>26</v>
+      </c>
+      <c r="F6" s="2"/>
+      <c r="G6" s="2"/>
+      <c r="H6" s="2"/>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>6</v>
       </c>
       <c r="B7" s="2">
-        <v>35.700000000000003</v>
+        <v>36</v>
       </c>
       <c r="C7" s="2">
-        <v>35.200000000000003</v>
+        <v>36</v>
       </c>
       <c r="D7" s="2">
-        <v>34.799999999999997</v>
+        <v>35</v>
       </c>
       <c r="E7" s="2">
-        <v>33.700000000000003</v>
-      </c>
-      <c r="F7" s="2">
-        <v>35.200000000000003</v>
-      </c>
-      <c r="G7" s="2">
-        <v>36.6</v>
-      </c>
-      <c r="H7" s="2">
-        <v>35.299999999999997</v>
-      </c>
+        <v>31</v>
+      </c>
+      <c r="F7" s="2"/>
+      <c r="G7" s="2"/>
+      <c r="H7" s="2"/>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>7</v>
       </c>
       <c r="B8" s="2">
-        <v>35</v>
+        <v>21</v>
       </c>
       <c r="C8" s="2">
-        <v>35.5</v>
+        <v>22</v>
       </c>
       <c r="D8" s="2">
-        <v>36.200000000000003</v>
+        <v>18</v>
       </c>
       <c r="E8" s="2">
-        <v>32.6</v>
-      </c>
-      <c r="F8" s="2">
-        <v>36.5</v>
-      </c>
-      <c r="G8" s="2">
-        <v>33.6</v>
-      </c>
-      <c r="H8" s="2">
-        <v>35.4</v>
-      </c>
+        <v>21</v>
+      </c>
+      <c r="F8" s="2"/>
+      <c r="G8" s="2"/>
+      <c r="H8" s="2"/>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>8</v>
       </c>
       <c r="B9" s="2">
-        <v>37</v>
+        <v>29</v>
       </c>
       <c r="C9" s="2">
-        <v>35.299999999999997</v>
+        <v>21</v>
       </c>
       <c r="D9" s="2">
-        <v>34.5</v>
+        <v>23</v>
       </c>
       <c r="E9" s="2">
-        <v>34.1</v>
-      </c>
-      <c r="F9" s="2">
-        <v>36.4</v>
-      </c>
-      <c r="G9" s="2">
-        <v>35.9</v>
-      </c>
-      <c r="H9" s="2">
-        <v>37.6</v>
-      </c>
+        <v>22</v>
+      </c>
+      <c r="F9" s="2"/>
+      <c r="G9" s="2"/>
+      <c r="H9" s="2"/>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>9</v>
       </c>
       <c r="B10" s="2">
-        <v>34.700000000000003</v>
+        <v>26</v>
       </c>
       <c r="C10" s="2">
-        <v>34.700000000000003</v>
+        <v>46</v>
       </c>
       <c r="D10" s="2">
-        <v>36.200000000000003</v>
+        <v>44</v>
       </c>
       <c r="E10" s="2">
-        <v>34.700000000000003</v>
-      </c>
-      <c r="F10" s="2">
-        <v>34.700000000000003</v>
-      </c>
-      <c r="G10" s="2">
-        <v>37.9</v>
-      </c>
-      <c r="H10" s="2">
-        <v>34</v>
-      </c>
+        <v>14</v>
+      </c>
+      <c r="F10" s="2"/>
+      <c r="G10" s="2"/>
+      <c r="H10" s="2"/>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>10</v>
       </c>
       <c r="B11" s="2">
-        <v>35.1</v>
+        <v>24</v>
       </c>
       <c r="C11" s="2">
-        <v>35.5</v>
+        <v>22</v>
       </c>
       <c r="D11" s="2">
+        <v>22</v>
+      </c>
+      <c r="E11" s="2">
+        <v>44</v>
+      </c>
+      <c r="F11" s="2"/>
+      <c r="G11" s="2"/>
+      <c r="H11" s="2"/>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A12">
+        <v>11</v>
+      </c>
+      <c r="B12" s="2">
+        <v>18</v>
+      </c>
+      <c r="C12" s="2">
+        <v>24</v>
+      </c>
+      <c r="D12" s="2">
+        <v>24</v>
+      </c>
+      <c r="E12" s="2">
+        <v>49</v>
+      </c>
+      <c r="F12" s="2"/>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A13">
+        <v>12</v>
+      </c>
+      <c r="B13" s="2">
+        <v>24</v>
+      </c>
+      <c r="C13" s="2">
+        <v>20</v>
+      </c>
+      <c r="D13" s="2">
+        <v>26</v>
+      </c>
+      <c r="E13" s="2">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A14">
+        <v>13</v>
+      </c>
+      <c r="B14" s="2">
+        <v>19</v>
+      </c>
+      <c r="C14" s="2">
+        <v>21</v>
+      </c>
+      <c r="D14" s="2">
+        <v>27</v>
+      </c>
+      <c r="E14" s="2">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A15">
+        <v>14</v>
+      </c>
+      <c r="B15" s="2">
+        <v>8</v>
+      </c>
+      <c r="C15" s="2">
+        <v>11</v>
+      </c>
+      <c r="D15" s="2">
+        <v>12</v>
+      </c>
+      <c r="E15" s="2">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A16">
+        <v>15</v>
+      </c>
+      <c r="B16" s="2">
+        <v>24</v>
+      </c>
+      <c r="C16" s="2">
+        <v>18.100000000000001</v>
+      </c>
+      <c r="D16" s="2">
+        <v>27</v>
+      </c>
+      <c r="E16" s="2">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A17">
+        <v>16</v>
+      </c>
+      <c r="B17" s="2">
+        <v>56</v>
+      </c>
+      <c r="C17" s="2">
+        <v>52</v>
+      </c>
+      <c r="D17" s="2">
+        <v>56</v>
+      </c>
+      <c r="E17" s="2">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A18">
+        <v>17</v>
+      </c>
+      <c r="B18" s="2">
+        <v>32.01</v>
+      </c>
+      <c r="C18" s="2">
+        <v>22</v>
+      </c>
+      <c r="D18" s="2">
+        <v>18</v>
+      </c>
+      <c r="E18" s="2">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A19">
+        <v>18</v>
+      </c>
+      <c r="B19" s="2">
+        <v>8</v>
+      </c>
+      <c r="C19" s="2">
+        <v>12.01</v>
+      </c>
+      <c r="D19" s="2">
+        <v>11</v>
+      </c>
+      <c r="E19" s="2">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A20">
+        <v>19</v>
+      </c>
+      <c r="B20" s="2">
+        <v>51</v>
+      </c>
+      <c r="C20" s="2">
+        <v>54</v>
+      </c>
+      <c r="D20" s="2">
+        <v>52.01</v>
+      </c>
+      <c r="E20" s="2">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A21">
+        <v>20</v>
+      </c>
+      <c r="B21" s="2">
+        <v>30</v>
+      </c>
+      <c r="C21" s="2">
+        <v>28</v>
+      </c>
+      <c r="D21" s="2">
         <v>35</v>
       </c>
-      <c r="E11" s="2">
-        <v>36.1</v>
-      </c>
-      <c r="F11" s="2">
-        <v>31.1</v>
-      </c>
-      <c r="G11" s="2">
-        <v>34.4</v>
-      </c>
-      <c r="H11" s="2">
-        <v>35.4</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="B12" s="2"/>
-      <c r="C12" s="2"/>
-      <c r="D12" s="2"/>
-      <c r="E12" s="2"/>
-      <c r="F12" s="2"/>
+      <c r="E21" s="2">
+        <v>22.01</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1002,10 +1097,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B11"/>
+  <dimension ref="A1:B21"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G31" sqref="G31"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1023,7 +1118,7 @@
         <v>1</v>
       </c>
       <c r="B2">
-        <v>3</v>
+        <v>12</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
@@ -1031,7 +1126,7 @@
         <v>2</v>
       </c>
       <c r="B3">
-        <v>5</v>
+        <v>14</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
@@ -1039,7 +1134,7 @@
         <v>3</v>
       </c>
       <c r="B4">
-        <v>2</v>
+        <v>16</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
@@ -1047,7 +1142,7 @@
         <v>4</v>
       </c>
       <c r="B5">
-        <v>5</v>
+        <v>18</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
@@ -1055,7 +1150,7 @@
         <v>5</v>
       </c>
       <c r="B6">
-        <v>9</v>
+        <v>16</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
@@ -1063,7 +1158,7 @@
         <v>6</v>
       </c>
       <c r="B7">
-        <v>4</v>
+        <v>14</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.3">
@@ -1071,7 +1166,7 @@
         <v>7</v>
       </c>
       <c r="B8">
-        <v>5</v>
+        <v>12</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.3">
@@ -1079,7 +1174,7 @@
         <v>8</v>
       </c>
       <c r="B9">
-        <v>2</v>
+        <v>12</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.3">
@@ -1087,7 +1182,7 @@
         <v>9</v>
       </c>
       <c r="B10">
-        <v>5</v>
+        <v>32</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.3">
@@ -1095,7 +1190,87 @@
         <v>10</v>
       </c>
       <c r="B11">
-        <v>3</v>
+        <v>16</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A12">
+        <v>11</v>
+      </c>
+      <c r="B12">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A13">
+        <v>12</v>
+      </c>
+      <c r="B13">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A14">
+        <v>13</v>
+      </c>
+      <c r="B14">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A15">
+        <v>14</v>
+      </c>
+      <c r="B15">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A16">
+        <v>15</v>
+      </c>
+      <c r="B16">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A17">
+        <v>16</v>
+      </c>
+      <c r="B17">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A18">
+        <v>17</v>
+      </c>
+      <c r="B18">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A19">
+        <v>18</v>
+      </c>
+      <c r="B19">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A20">
+        <v>19</v>
+      </c>
+      <c r="B20">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A21">
+        <v>20</v>
+      </c>
+      <c r="B21">
+        <v>21</v>
       </c>
     </row>
   </sheetData>
@@ -1599,7 +1774,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="I15" sqref="I15"/>
     </sheetView>
   </sheetViews>

</xml_diff>